<commit_message>
FOM cost updated for coal power plant
</commit_message>
<xml_diff>
--- a/VT_REGION1_PWR.xlsx
+++ b/VT_REGION1_PWR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\minimodel2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BB631E-5778-4022-A850-F5C10981E0BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6EC83B-8F45-4F28-9D58-DD03D2F0DA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4005" yWindow="1545" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{37FD0756-6F24-4C61-AC4B-6F35E5E0357A}"/>
   </bookViews>
@@ -1831,7 +1831,7 @@
   <dimension ref="C3:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1962,7 +1962,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="22">
-        <v>10</v>
+        <v>600</v>
       </c>
       <c r="K7" s="22">
         <v>50000</v>

</xml_diff>

<commit_message>
with wind and PV 24 TS
</commit_message>
<xml_diff>
--- a/VT_REGION1_PWR.xlsx
+++ b/VT_REGION1_PWR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\minimodel2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6EC83B-8F45-4F28-9D58-DD03D2F0DA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FB51A3-65F6-433B-B024-A7B36AC2EFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4005" yWindow="1545" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{37FD0756-6F24-4C61-AC4B-6F35E5E0357A}"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="28800" windowHeight="15570" activeTab="1" xr2:uid="{37FD0756-6F24-4C61-AC4B-6F35E5E0357A}"/>
   </bookViews>
   <sheets>
     <sheet name="SATIM-EL" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="95">
   <si>
     <t>Primary Supply</t>
   </si>
@@ -125,9 +125,6 @@
     <t>EHYDGeneric</t>
   </si>
   <si>
-    <t>Wind/Solar Power Plants</t>
-  </si>
-  <si>
     <t>EWNDGeneric</t>
   </si>
   <si>
@@ -309,6 +306,24 @@
   </si>
   <si>
     <t>Demand</t>
+  </si>
+  <si>
+    <t>Wind Power</t>
+  </si>
+  <si>
+    <t>Solar Power</t>
+  </si>
+  <si>
+    <t>Wind Power Plants</t>
+  </si>
+  <si>
+    <t>Solar Power Plants</t>
+  </si>
+  <si>
+    <t>EPVCGeneric</t>
+  </si>
+  <si>
+    <t>PV Centralized</t>
   </si>
 </sst>
 </file>
@@ -373,6 +388,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -490,7 +506,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -589,15 +605,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -665,8 +672,8 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -699,9 +706,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -738,18 +745,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1193,10 +1188,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC812D5-4A4E-4049-BBCC-4AA023FE6DD9}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="C1:O25"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1472,7 +1468,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="14"/>
       <c r="H17" s="7" t="s">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="I17" s="5"/>
       <c r="K17" s="1"/>
@@ -1484,7 +1480,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="14"/>
       <c r="H18" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I18" s="14"/>
       <c r="K18" s="1"/>
@@ -1503,7 +1499,10 @@
     </row>
     <row r="20" spans="3:15" x14ac:dyDescent="0.25">
       <c r="F20" s="14"/>
-      <c r="I20" s="4"/>
+      <c r="H20" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I20" s="5"/>
       <c r="K20" s="1"/>
       <c r="L20" s="4"/>
       <c r="N20" s="1"/>
@@ -1511,12 +1510,15 @@
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C21" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
-      <c r="I21" s="4"/>
+      <c r="H21" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I21" s="14"/>
       <c r="K21" s="1"/>
       <c r="L21" s="4"/>
       <c r="N21" s="1"/>
@@ -1524,7 +1526,7 @@
     </row>
     <row r="22" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C22" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="4"/>
@@ -1570,10 +1572,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E32065-2787-45F4-A450-6CE2DA6FE842}">
-  <dimension ref="C3:H22"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="C3:O16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,243 +1585,274 @@
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C3" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="15"/>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C4" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="15"/>
-    </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="15" t="s">
+      <c r="D4" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="E4" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="F4" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="G4" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="H4" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="O4" s="16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="19" t="s">
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" t="s">
         <v>1</v>
       </c>
       <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" t="s">
         <v>50</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="16"/>
+      <c r="N5" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
+        <v>52</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
         <v>51</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="J9" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K10" t="s">
+        <v>44</v>
+      </c>
+      <c r="L10" t="s">
+        <v>45</v>
+      </c>
+      <c r="M10" t="s">
+        <v>46</v>
+      </c>
+      <c r="N10" t="s">
+        <v>47</v>
+      </c>
+      <c r="O10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11" t="s">
+        <v>49</v>
+      </c>
+      <c r="M11" t="s">
+        <v>54</v>
+      </c>
+      <c r="N11" t="s">
+        <v>52</v>
+      </c>
+      <c r="O11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" t="s">
+        <v>49</v>
+      </c>
+      <c r="M12" t="s">
+        <v>55</v>
+      </c>
+      <c r="N12" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="O12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" t="s">
+        <v>49</v>
+      </c>
+      <c r="M13" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="H12" s="16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D13" s="16"/>
-      <c r="G13" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="F14" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="E15" s="16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C18" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="G18" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="H18" s="18" t="s">
+      <c r="N13" t="s">
+        <v>53</v>
+      </c>
+      <c r="O13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C19" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="M14" t="s">
         <v>55</v>
       </c>
-      <c r="G19" t="s">
+      <c r="N14" t="s">
         <v>53</v>
       </c>
-      <c r="H19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" t="s">
-        <v>50</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="O14" t="s">
         <v>56</v>
       </c>
-      <c r="G20" t="s">
-        <v>54</v>
-      </c>
-      <c r="H20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" t="s">
-        <v>50</v>
-      </c>
-      <c r="F21" t="s">
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>28</v>
+      </c>
+      <c r="K15" t="s">
+        <v>89</v>
+      </c>
+      <c r="L15" t="s">
+        <v>49</v>
+      </c>
+      <c r="M15" t="s">
+        <v>55</v>
+      </c>
+      <c r="N15" t="s">
+        <v>53</v>
+      </c>
+      <c r="O15" t="s">
         <v>56</v>
       </c>
-      <c r="G21" t="s">
-        <v>54</v>
-      </c>
-      <c r="H21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" t="s">
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>93</v>
+      </c>
+      <c r="K16" t="s">
+        <v>90</v>
+      </c>
+      <c r="L16" t="s">
+        <v>49</v>
+      </c>
+      <c r="M16" t="s">
         <v>55</v>
       </c>
-      <c r="G22" t="s">
-        <v>54</v>
-      </c>
-      <c r="H22" t="s">
-        <v>58</v>
+      <c r="N16" t="s">
+        <v>53</v>
+      </c>
+      <c r="O16" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1828,10 +1862,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF44DDC-D079-43BE-BBFD-41A34FD9B05F}">
-  <dimension ref="C3:N10"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="C3:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1844,212 +1879,258 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22" t="s">
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+    </row>
+    <row r="4" spans="3:14" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="C4" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-    </row>
-    <row r="4" spans="3:14" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="C4" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="G4" s="26" t="s">
+      <c r="I4" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="H4" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="I4" s="27" t="s">
+      <c r="J4" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="J4" s="27" t="s">
+      <c r="K4" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="K4" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="L4" s="27" t="s">
+      <c r="M4" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="M4" s="27" t="s">
+      <c r="N4" s="23" t="s">
         <v>68</v>
-      </c>
-      <c r="N4" s="27" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="5" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" t="s">
         <v>71</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>72</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>73</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>74</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>75</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>76</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>77</v>
-      </c>
-      <c r="K5" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="6" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I6" t="s">
         <v>79</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>80</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
+        <v>80</v>
+      </c>
+      <c r="L6" t="s">
         <v>81</v>
       </c>
-      <c r="K6" t="s">
-        <v>81</v>
-      </c>
-      <c r="L6" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C7" s="23" t="str">
+      <c r="C7" t="str">
+        <f>'SATIM-EL'!C8</f>
+        <v>MINCLE</v>
+      </c>
+      <c r="D7" t="str">
+        <f>'SATIM-EL'!C7</f>
+        <v>Coal Mines</v>
+      </c>
+      <c r="F7" t="str">
+        <f>E10</f>
+        <v>CLE</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>35</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C8" t="str">
+        <f>'SATIM-EL'!K7</f>
+        <v>ETRANS</v>
+      </c>
+      <c r="D8" t="str">
+        <f>'SATIM-EL'!K6</f>
+        <v>Electricity Network</v>
+      </c>
+      <c r="E8" t="str">
+        <f>F10</f>
+        <v>ELCC</v>
+      </c>
+      <c r="F8" t="str">
+        <f>'SATIM-EL'!L2</f>
+        <v>ELC</v>
+      </c>
+      <c r="H8">
+        <v>0.88</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <f>M10</f>
+        <v>31.536000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C9" t="str">
+        <f>'SATIM-EL'!N7</f>
+        <v>RDEM</v>
+      </c>
+      <c r="D9" t="str">
+        <f>'SATIM-EL'!N6</f>
+        <v>Demand Technology</v>
+      </c>
+      <c r="E9" t="str">
+        <f>F8</f>
+        <v>ELC</v>
+      </c>
+      <c r="F9" t="str">
+        <f>'SATIM-EL'!O2</f>
+        <v>RDEM1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C10" s="19" t="str">
         <f>'SATIM-EL'!H6</f>
         <v>ETCLEGeneric</v>
       </c>
-      <c r="D7" s="22" t="str">
+      <c r="D10" s="18" t="str">
         <f>'SATIM-EL'!H5</f>
         <v>Coal Power Plants</v>
       </c>
-      <c r="E7" s="22" t="str">
+      <c r="E10" s="18" t="str">
         <f>'SATIM-EL'!E2</f>
         <v>CLE</v>
       </c>
-      <c r="F7" s="22" t="str">
+      <c r="F10" s="18" t="str">
         <f>'SATIM-EL'!I2</f>
         <v>ELCC</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H10" s="18">
         <v>0.35</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I10" s="18">
         <v>1</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J10" s="18">
         <v>600</v>
       </c>
-      <c r="K7" s="22">
+      <c r="K10" s="18">
         <v>50000</v>
       </c>
-      <c r="L7" s="22">
+      <c r="L10" s="18">
         <v>30</v>
       </c>
-      <c r="M7" s="22">
+      <c r="M10" s="18">
         <v>31.536000000000001</v>
       </c>
-      <c r="N7" s="22">
+      <c r="N10" s="18">
         <v>0.7</v>
       </c>
     </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C8" t="str">
-        <f>'SATIM-EL'!C8</f>
-        <v>MINCLE</v>
-      </c>
-      <c r="D8" t="str">
-        <f>'SATIM-EL'!C7</f>
-        <v>Coal Mines</v>
-      </c>
-      <c r="F8" t="str">
-        <f>E7</f>
-        <v>CLE</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>35</v>
-      </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C9" t="str">
-        <f>'SATIM-EL'!K7</f>
-        <v>ETRANS</v>
-      </c>
-      <c r="D9" t="str">
-        <f>'SATIM-EL'!K6</f>
-        <v>Electricity Network</v>
-      </c>
-      <c r="E9" t="str">
-        <f>F7</f>
-        <v>ELCC</v>
-      </c>
-      <c r="F9" t="str">
-        <f>'SATIM-EL'!L2</f>
-        <v>ELC</v>
-      </c>
-      <c r="H9">
-        <v>0.88</v>
-      </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="M9">
-        <f>M7</f>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11">
+        <v>860</v>
+      </c>
+      <c r="K11">
+        <v>17000</v>
+      </c>
+      <c r="L11">
+        <v>20</v>
+      </c>
+      <c r="M11" s="18">
         <v>31.536000000000001</v>
       </c>
     </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C10" t="str">
-        <f>'SATIM-EL'!N7</f>
-        <v>RDEM</v>
-      </c>
-      <c r="D10" t="str">
-        <f>'SATIM-EL'!N6</f>
-        <v>Demand Technology</v>
-      </c>
-      <c r="E10" t="str">
-        <f>F9</f>
-        <v>ELC</v>
-      </c>
-      <c r="F10" t="str">
-        <f>'SATIM-EL'!O2</f>
-        <v>RDEM1</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="M10">
-        <v>1</v>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12">
+        <v>380</v>
+      </c>
+      <c r="K12">
+        <v>14000</v>
+      </c>
+      <c r="L12">
+        <v>25</v>
+      </c>
+      <c r="M12" s="18">
+        <v>31.536000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2059,6 +2140,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18519367-7B9C-4CF2-B542-D2BDFD86BE47}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="C3:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2073,61 +2155,61 @@
     <row r="3" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C3" s="15"/>
       <c r="D3" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C4" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>83</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>84</v>
       </c>
       <c r="F4" s="15">
         <v>2017</v>
       </c>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C5" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="29" t="s">
+      <c r="C5" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="F5" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="F5" s="29" t="s">
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="24" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="28" t="s">
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="29" t="str">
+      <c r="D7" s="25" t="str">
         <f>'SATIM-EL'!O2</f>
         <v>RDEM1</v>
       </c>
-      <c r="E7" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="30">
+      <c r="E7" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="26">
         <f>200*3.6</f>
         <v>720</v>
       </c>

</xml_diff>

<commit_message>
some small fixes incl. RPT_OPT
</commit_message>
<xml_diff>
--- a/VT_REGION1_PWR.xlsx
+++ b/VT_REGION1_PWR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\minimodel2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FB51A3-65F6-433B-B024-A7B36AC2EFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CAD4673-DA5D-4A53-BA57-5E1021ABBF22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="28800" windowHeight="15570" activeTab="1" xr2:uid="{37FD0756-6F24-4C61-AC4B-6F35E5E0357A}"/>
+    <workbookView xWindow="-1350" yWindow="-17670" windowWidth="28800" windowHeight="15570" activeTab="3" xr2:uid="{37FD0756-6F24-4C61-AC4B-6F35E5E0357A}"/>
   </bookViews>
   <sheets>
     <sheet name="SATIM-EL" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="95">
   <si>
     <t>Primary Supply</t>
   </si>
@@ -1575,8 +1575,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="C3:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1674,6 +1674,9 @@
       <c r="G7" t="s">
         <v>53</v>
       </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
       <c r="L7" s="16" t="s">
         <v>41</v>
       </c>
@@ -1693,6 +1696,9 @@
       </c>
       <c r="G8" t="s">
         <v>53</v>
+      </c>
+      <c r="H8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="3:15" x14ac:dyDescent="0.25">
@@ -2143,8 +2149,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="C3:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2210,8 +2216,8 @@
         <v>49</v>
       </c>
       <c r="F7" s="26">
-        <f>200*3.6</f>
-        <v>720</v>
+        <f>235*3.6</f>
+        <v>846</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
with 2 seasons + Battery Storage
</commit_message>
<xml_diff>
--- a/VT_REGION1_PWR.xlsx
+++ b/VT_REGION1_PWR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\minimodel2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CAD4673-DA5D-4A53-BA57-5E1021ABBF22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0595EF-715B-4E99-A582-D865C8A76E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1350" yWindow="-17670" windowWidth="28800" windowHeight="15570" activeTab="3" xr2:uid="{37FD0756-6F24-4C61-AC4B-6F35E5E0357A}"/>
+    <workbookView xWindow="-1440" yWindow="-17700" windowWidth="28800" windowHeight="15570" activeTab="2" xr2:uid="{37FD0756-6F24-4C61-AC4B-6F35E5E0357A}"/>
   </bookViews>
   <sheets>
     <sheet name="SATIM-EL" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="100">
   <si>
     <t>Primary Supply</t>
   </si>
@@ -308,12 +308,6 @@
     <t>Demand</t>
   </si>
   <si>
-    <t>Wind Power</t>
-  </si>
-  <si>
-    <t>Solar Power</t>
-  </si>
-  <si>
     <t>Wind Power Plants</t>
   </si>
   <si>
@@ -323,17 +317,39 @@
     <t>EPVCGeneric</t>
   </si>
   <si>
-    <t>PV Centralized</t>
+    <t>Discount Rate</t>
+  </si>
+  <si>
+    <t>LCOE</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>PRE,STGTSS</t>
+  </si>
+  <si>
+    <t>STG_EFF</t>
+  </si>
+  <si>
+    <t>Storage Efficiency</t>
+  </si>
+  <si>
+    <t>NCAP_AFC</t>
+  </si>
+  <si>
+    <t>Storage hours</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="\Te\x\t"/>
     <numFmt numFmtId="165" formatCode="[$£-809]#,##0.000;[Red]&quot;-&quot;[$£-809]#,##0.000"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -635,7 +651,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="65">
+  <cellStyleXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -707,8 +723,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -762,11 +779,21 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="65" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="65" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="65">
+  <cellStyles count="66">
     <cellStyle name="20% - Accent5 2" xfId="43" xr:uid="{D6EEBD42-F946-4489-B3C1-5EB6FE66A95B}"/>
     <cellStyle name="60% - Accent2 2" xfId="44" xr:uid="{531AF5E1-A27A-4718-959A-A677CE7C5310}"/>
     <cellStyle name="Calculation 2" xfId="33" xr:uid="{4D7D19EC-A7F2-4E38-A3A4-9345E5346D99}"/>
+    <cellStyle name="Comma" xfId="65" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="9" xr:uid="{73794E6E-A261-4680-AF00-F7823E1C65E7}"/>
     <cellStyle name="Comma 2 2" xfId="17" xr:uid="{B02737DE-2325-4C14-820E-8AFC03B3DDAC}"/>
     <cellStyle name="Comma 2 2 2" xfId="31" xr:uid="{9FEE4DD9-2287-416A-8178-102898EDA9FF}"/>
@@ -1192,7 +1219,7 @@
   <dimension ref="C1:O25"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,7 +1404,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="1"/>
-      <c r="I10" s="4"/>
+      <c r="I10" s="6"/>
       <c r="K10" s="1"/>
       <c r="L10" s="4"/>
       <c r="N10" s="1"/>
@@ -1392,7 +1419,7 @@
       <c r="H11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="5"/>
+      <c r="I11" s="14"/>
       <c r="K11" s="1"/>
       <c r="L11" s="4"/>
       <c r="N11" s="1"/>
@@ -1407,7 +1434,7 @@
       <c r="H12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="4"/>
+      <c r="I12" s="5"/>
       <c r="K12" s="1"/>
       <c r="L12" s="4"/>
       <c r="N12" s="1"/>
@@ -1468,7 +1495,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="14"/>
       <c r="H17" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I17" s="5"/>
       <c r="K17" s="1"/>
@@ -1500,7 +1527,7 @@
     <row r="20" spans="3:15" x14ac:dyDescent="0.25">
       <c r="F20" s="14"/>
       <c r="H20" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I20" s="5"/>
       <c r="K20" s="1"/>
@@ -1516,7 +1543,7 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="H21" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I21" s="14"/>
       <c r="K21" s="1"/>
@@ -1573,10 +1600,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E32065-2787-45F4-A450-6CE2DA6FE842}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="C3:O16"/>
+  <dimension ref="C3:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="L18" sqref="L18:M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,6 +1613,7 @@
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" customWidth="1"/>
     <col min="10" max="10" width="14.140625" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:15" x14ac:dyDescent="0.25">
@@ -1763,70 +1791,71 @@
     </row>
     <row r="12" spans="3:15" x14ac:dyDescent="0.25">
       <c r="J12" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="K12" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="L12" t="s">
         <v>49</v>
       </c>
       <c r="M12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N12" t="s">
         <v>53</v>
       </c>
       <c r="O12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="3:15" x14ac:dyDescent="0.25">
       <c r="J13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L13" t="s">
         <v>49</v>
       </c>
       <c r="M13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="N13" t="s">
         <v>53</v>
       </c>
       <c r="O13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="3:15" x14ac:dyDescent="0.25">
       <c r="J14" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="K14" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L14" t="s">
         <v>49</v>
       </c>
       <c r="M14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N14" t="s">
         <v>53</v>
       </c>
       <c r="O14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="3:15" x14ac:dyDescent="0.25">
       <c r="J15" t="s">
-        <v>28</v>
-      </c>
-      <c r="K15" t="s">
-        <v>89</v>
+        <v>15</v>
+      </c>
+      <c r="K15" t="str">
+        <f>'SATIM-EL'!H5</f>
+        <v>Coal Power Plants</v>
       </c>
       <c r="L15" t="s">
         <v>49</v>
@@ -1843,10 +1872,11 @@
     </row>
     <row r="16" spans="3:15" x14ac:dyDescent="0.25">
       <c r="J16" t="s">
-        <v>93</v>
-      </c>
-      <c r="K16" t="s">
-        <v>90</v>
+        <v>23</v>
+      </c>
+      <c r="K16" t="str">
+        <f>'SATIM-EL'!H8</f>
+        <v>Gas Power Plants</v>
       </c>
       <c r="L16" t="s">
         <v>49</v>
@@ -1859,6 +1889,70 @@
       </c>
       <c r="O16" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" t="str">
+        <f>'SATIM-EL'!H17</f>
+        <v>Wind Power Plants</v>
+      </c>
+      <c r="L17" t="s">
+        <v>49</v>
+      </c>
+      <c r="M17" t="s">
+        <v>55</v>
+      </c>
+      <c r="N17" t="s">
+        <v>53</v>
+      </c>
+      <c r="O17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K18" t="str">
+        <f>'SATIM-EL'!H20</f>
+        <v>Solar Power Plants</v>
+      </c>
+      <c r="L18" t="s">
+        <v>49</v>
+      </c>
+      <c r="M18" t="s">
+        <v>55</v>
+      </c>
+      <c r="N18" t="s">
+        <v>53</v>
+      </c>
+      <c r="O18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J19" t="str">
+        <f>'SATIM-EL'!H12</f>
+        <v>ESTGeneric</v>
+      </c>
+      <c r="K19" t="str">
+        <f>'SATIM-EL'!H11</f>
+        <v>Battery</v>
+      </c>
+      <c r="L19" t="s">
+        <v>49</v>
+      </c>
+      <c r="M19" t="s">
+        <v>55</v>
+      </c>
+      <c r="N19" t="s">
+        <v>53</v>
+      </c>
+      <c r="O19" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1869,22 +1963,30 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF44DDC-D079-43BE-BBFD-41A34FD9B05F}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="C3:N12"/>
+  <dimension ref="C1:T15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>92</v>
+      </c>
+      <c r="T1" s="29">
+        <v>8.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="3:20" x14ac:dyDescent="0.25">
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
@@ -1897,8 +1999,10 @@
       <c r="K3" s="18"/>
       <c r="L3" s="18"/>
       <c r="M3" s="18"/>
-    </row>
-    <row r="4" spans="3:14" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+    </row>
+    <row r="4" spans="3:20" ht="23.25" x14ac:dyDescent="0.25">
       <c r="C4" s="21" t="s">
         <v>43</v>
       </c>
@@ -1917,26 +2021,38 @@
       <c r="H4" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="K4" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="J4" s="23" t="s">
+      <c r="L4" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="K4" s="23" t="s">
+      <c r="M4" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="L4" s="23" t="s">
+      <c r="N4" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="M4" s="23" t="s">
+      <c r="O4" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="N4" s="23" t="s">
+      <c r="P4" s="23" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="S4" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="T4" s="30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>70</v>
       </c>
@@ -1953,33 +2069,39 @@
         <v>74</v>
       </c>
       <c r="I5" t="s">
+        <v>97</v>
+      </c>
+      <c r="J5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K5" t="s">
         <v>75</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>76</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>78</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>79</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>80</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>80</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C7" t="str">
         <f>'SATIM-EL'!C8</f>
         <v>MINCLE</v>
@@ -1989,153 +2111,274 @@
         <v>Coal Mines</v>
       </c>
       <c r="F7" t="str">
-        <f>E10</f>
+        <f>E11</f>
         <v>CLE</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>35</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C8" t="str">
+        <f>'SATIM-EL'!C22</f>
+        <v>IMPGAS</v>
+      </c>
+      <c r="D8" t="str">
+        <f>'SATIM-EL'!C21</f>
+        <v>Gas Imports</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>272</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C9" t="str">
         <f>'SATIM-EL'!K7</f>
         <v>ETRANS</v>
       </c>
-      <c r="D8" t="str">
+      <c r="D9" t="str">
         <f>'SATIM-EL'!K6</f>
         <v>Electricity Network</v>
       </c>
-      <c r="E8" t="str">
-        <f>F10</f>
+      <c r="E9" t="str">
+        <f>F11</f>
         <v>ELCC</v>
       </c>
-      <c r="F8" t="str">
+      <c r="F9" t="str">
         <f>'SATIM-EL'!L2</f>
         <v>ELC</v>
       </c>
-      <c r="H8">
+      <c r="H9">
         <v>0.88</v>
       </c>
-      <c r="K8">
+      <c r="M9">
         <v>1</v>
       </c>
-      <c r="M8">
-        <f>M10</f>
+      <c r="O9">
+        <f>O11</f>
         <v>31.536000000000001</v>
       </c>
     </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C9" t="str">
+    <row r="10" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C10" t="str">
         <f>'SATIM-EL'!N7</f>
         <v>RDEM</v>
       </c>
-      <c r="D9" t="str">
+      <c r="D10" t="str">
         <f>'SATIM-EL'!N6</f>
         <v>Demand Technology</v>
       </c>
-      <c r="E9" t="str">
-        <f>F8</f>
+      <c r="E10" t="str">
+        <f>F9</f>
         <v>ELC</v>
       </c>
-      <c r="F9" t="str">
+      <c r="F10" t="str">
         <f>'SATIM-EL'!O2</f>
         <v>RDEM1</v>
       </c>
-      <c r="H9">
+      <c r="H10">
         <v>1</v>
       </c>
-      <c r="M9">
+      <c r="O10">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C10" s="19" t="str">
+    <row r="11" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C11" s="19" t="str">
         <f>'SATIM-EL'!H6</f>
         <v>ETCLEGeneric</v>
       </c>
-      <c r="D10" s="18" t="str">
+      <c r="D11" s="18" t="str">
         <f>'SATIM-EL'!H5</f>
         <v>Coal Power Plants</v>
       </c>
-      <c r="E10" s="18" t="str">
+      <c r="E11" s="18" t="str">
         <f>'SATIM-EL'!E2</f>
         <v>CLE</v>
       </c>
-      <c r="F10" s="18" t="str">
+      <c r="F11" s="18" t="str">
         <f>'SATIM-EL'!I2</f>
         <v>ELCC</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H11" s="18">
         <v>0.35</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18">
         <v>1</v>
       </c>
-      <c r="J10" s="18">
-        <v>600</v>
-      </c>
-      <c r="K10" s="18">
+      <c r="L11" s="18">
+        <v>1000</v>
+      </c>
+      <c r="M11" s="27">
         <v>50000</v>
       </c>
-      <c r="L10" s="18">
+      <c r="N11" s="18">
         <v>30</v>
       </c>
-      <c r="M10" s="18">
+      <c r="O11" s="18">
         <v>31.536000000000001</v>
       </c>
-      <c r="N10" s="18">
+      <c r="P11" s="18">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+      <c r="S11">
+        <f>P11</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="12" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C12" s="19" t="str">
+        <f>'SATIM-EL'!H9</f>
+        <v>ETGASGeneric</v>
+      </c>
+      <c r="D12" s="18" t="str">
+        <f>'SATIM-EL'!H8</f>
+        <v>Gas Power Plants</v>
+      </c>
+      <c r="E12" s="18" t="str">
+        <f>'SATIM-EL'!F2</f>
+        <v>GAS</v>
+      </c>
+      <c r="F12" s="18" t="str">
+        <f>F11</f>
+        <v>ELCC</v>
+      </c>
+      <c r="H12" s="18">
+        <v>0.35</v>
+      </c>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18">
+        <v>1</v>
+      </c>
+      <c r="L12" s="18">
+        <v>100</v>
+      </c>
+      <c r="M12" s="27">
+        <v>15000</v>
+      </c>
+      <c r="N12" s="18">
+        <v>30</v>
+      </c>
+      <c r="O12" s="18">
+        <v>31.536000000000001</v>
+      </c>
+      <c r="P12" s="18">
+        <v>0.9</v>
+      </c>
+      <c r="S12">
+        <f>P12</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="13" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
         <v>28</v>
       </c>
-      <c r="D11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="D13" t="str">
+        <f>'SATIM-EL'!H17</f>
+        <v>Wind Power Plants</v>
+      </c>
+      <c r="F13" t="s">
         <v>11</v>
       </c>
-      <c r="J11">
-        <v>860</v>
-      </c>
-      <c r="K11">
-        <v>17000</v>
-      </c>
-      <c r="L11">
+      <c r="L13">
+        <v>955</v>
+      </c>
+      <c r="M13" s="28">
+        <v>25000</v>
+      </c>
+      <c r="N13">
         <v>20</v>
       </c>
-      <c r="M11" s="18">
+      <c r="O13" s="18">
         <v>31.536000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>93</v>
-      </c>
-      <c r="D12" t="s">
-        <v>94</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="S13">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="T13" s="31">
+        <f>(-PMT($T$1,N13,1,0,1)*M13+L13)/S13</f>
+        <v>94.715730649564591</v>
+      </c>
+    </row>
+    <row r="14" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" t="str">
+        <f>'SATIM-EL'!H20</f>
+        <v>Solar Power Plants</v>
+      </c>
+      <c r="F14" t="s">
         <v>11</v>
       </c>
-      <c r="J12">
-        <v>380</v>
-      </c>
-      <c r="K12">
+      <c r="L14">
+        <v>295</v>
+      </c>
+      <c r="M14" s="28">
         <v>14000</v>
       </c>
-      <c r="L12">
+      <c r="N14">
         <v>25</v>
       </c>
-      <c r="M12" s="18">
+      <c r="O14" s="18">
+        <v>31.536000000000001</v>
+      </c>
+      <c r="S14">
+        <v>29.4</v>
+      </c>
+      <c r="T14" s="31">
+        <f>(-PMT($T$1,N14,1,0,1)*M14+L14)/S14</f>
+        <v>51.968852532769347</v>
+      </c>
+    </row>
+    <row r="15" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C15" t="str">
+        <f>Declarations!J19</f>
+        <v>ESTGeneric</v>
+      </c>
+      <c r="D15" t="str">
+        <f>Declarations!K19</f>
+        <v>Battery</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15">
+        <v>0.89</v>
+      </c>
+      <c r="J15">
+        <f>4/24</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M15">
+        <v>19444</v>
+      </c>
+      <c r="N15">
+        <v>15</v>
+      </c>
+      <c r="O15" s="18">
         <v>31.536000000000001</v>
       </c>
     </row>
@@ -2149,7 +2392,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="C3:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Battery Storage adjusted and hourly TS params added
</commit_message>
<xml_diff>
--- a/VT_REGION1_PWR.xlsx
+++ b/VT_REGION1_PWR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\minimodel2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0595EF-715B-4E99-A582-D865C8A76E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BC50C3-CC69-4612-93DB-2E8F50E43F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1440" yWindow="-17700" windowWidth="28800" windowHeight="15570" activeTab="2" xr2:uid="{37FD0756-6F24-4C61-AC4B-6F35E5E0357A}"/>
+    <workbookView xWindow="-1845" yWindow="-18225" windowWidth="28800" windowHeight="15570" activeTab="2" xr2:uid="{37FD0756-6F24-4C61-AC4B-6F35E5E0357A}"/>
   </bookViews>
   <sheets>
     <sheet name="SATIM-EL" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="104">
   <si>
     <t>Primary Supply</t>
   </si>
@@ -326,19 +326,31 @@
     <t>CF</t>
   </si>
   <si>
-    <t>PRE,STGTSS</t>
-  </si>
-  <si>
     <t>STG_EFF</t>
   </si>
   <si>
     <t>Storage Efficiency</t>
   </si>
   <si>
-    <t>NCAP_AFC</t>
-  </si>
-  <si>
     <t>Storage hours</t>
+  </si>
+  <si>
+    <t>ELE,STG</t>
+  </si>
+  <si>
+    <t>PrimaryCG</t>
+  </si>
+  <si>
+    <t>ACT</t>
+  </si>
+  <si>
+    <t>Annualized inv</t>
+  </si>
+  <si>
+    <t>FLO_SHAR~UP</t>
+  </si>
+  <si>
+    <t>AFC~DAYNITE</t>
   </si>
 </sst>
 </file>
@@ -784,10 +796,8 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="65" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="20% - Accent5 2" xfId="43" xr:uid="{D6EEBD42-F946-4489-B3C1-5EB6FE66A95B}"/>
@@ -1600,10 +1610,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E32065-2787-45F4-A450-6CE2DA6FE842}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="C3:O19"/>
+  <dimension ref="C3:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18:M19"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1616,13 +1626,13 @@
     <col min="11" max="11" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C3" s="15" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="15"/>
     </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C4" s="15" t="s">
         <v>32</v>
       </c>
@@ -1645,7 +1655,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>9</v>
       </c>
@@ -1666,7 +1676,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>10</v>
       </c>
@@ -1686,7 +1696,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>11</v>
       </c>
@@ -1709,7 +1719,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>12</v>
       </c>
@@ -1729,7 +1739,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>13</v>
       </c>
@@ -1749,7 +1759,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
         <v>43</v>
       </c>
@@ -1768,8 +1778,11 @@
       <c r="O10" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
       <c r="J11" t="s">
         <v>21</v>
       </c>
@@ -1789,7 +1802,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="J12" t="s">
         <v>30</v>
       </c>
@@ -1809,7 +1822,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
       <c r="J13" t="s">
         <v>19</v>
       </c>
@@ -1829,7 +1842,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
       <c r="J14" t="s">
         <v>20</v>
       </c>
@@ -1849,7 +1862,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
       <c r="J15" t="s">
         <v>15</v>
       </c>
@@ -1870,7 +1883,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
       <c r="J16" t="s">
         <v>23</v>
       </c>
@@ -1891,7 +1904,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
         <v>28</v>
       </c>
@@ -1912,7 +1925,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J18" t="s">
         <v>91</v>
       </c>
@@ -1933,7 +1946,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J19" t="str">
         <f>'SATIM-EL'!H12</f>
         <v>ESTGeneric</v>
@@ -1952,7 +1965,10 @@
         <v>53</v>
       </c>
       <c r="O19" t="s">
-        <v>95</v>
+        <v>98</v>
+      </c>
+      <c r="P19" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1963,10 +1979,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF44DDC-D079-43BE-BBFD-41A34FD9B05F}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="C1:T15"/>
+  <dimension ref="C1:Z16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1976,17 +1992,19 @@
     <col min="13" max="13" width="11.42578125" customWidth="1"/>
     <col min="14" max="14" width="11.140625" customWidth="1"/>
     <col min="15" max="15" width="12.140625" customWidth="1"/>
+    <col min="20" max="20" width="11.140625" customWidth="1"/>
+    <col min="21" max="25" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="R1" t="s">
+    <row r="1" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="S1" t="s">
         <v>92</v>
       </c>
-      <c r="T1" s="29">
+      <c r="U1" s="29">
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="3" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:26" x14ac:dyDescent="0.25">
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
@@ -2002,7 +2020,7 @@
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
     </row>
-    <row r="4" spans="3:20" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:26" ht="23.25" x14ac:dyDescent="0.25">
       <c r="C4" s="21" t="s">
         <v>43</v>
       </c>
@@ -2022,10 +2040,10 @@
         <v>60</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="J4" s="20" t="s">
-        <v>98</v>
+        <v>95</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>103</v>
       </c>
       <c r="K4" s="23" t="s">
         <v>64</v>
@@ -2045,14 +2063,20 @@
       <c r="P4" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="S4" s="30" t="s">
+      <c r="Q4" t="s">
+        <v>102</v>
+      </c>
+      <c r="T4" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="T4" s="30" t="s">
+      <c r="U4" s="23" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="5" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V4" s="23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>70</v>
       </c>
@@ -2069,10 +2093,10 @@
         <v>74</v>
       </c>
       <c r="I5" t="s">
+        <v>96</v>
+      </c>
+      <c r="J5" t="s">
         <v>97</v>
-      </c>
-      <c r="J5" t="s">
-        <v>99</v>
       </c>
       <c r="K5" t="s">
         <v>75</v>
@@ -2084,7 +2108,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>78</v>
       </c>
@@ -2101,7 +2125,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C7" t="str">
         <f>'SATIM-EL'!C8</f>
         <v>MINCLE</v>
@@ -2124,7 +2148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C8" t="str">
         <f>'SATIM-EL'!C22</f>
         <v>IMPGAS</v>
@@ -2146,7 +2170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C9" t="str">
         <f>'SATIM-EL'!K7</f>
         <v>ETRANS</v>
@@ -2174,7 +2198,7 @@
         <v>31.536000000000001</v>
       </c>
     </row>
-    <row r="10" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C10" t="str">
         <f>'SATIM-EL'!N7</f>
         <v>RDEM</v>
@@ -2198,7 +2222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C11" s="19" t="str">
         <f>'SATIM-EL'!H6</f>
         <v>ETCLEGeneric</v>
@@ -2224,10 +2248,10 @@
         <v>1</v>
       </c>
       <c r="L11" s="18">
-        <v>1000</v>
+        <v>1439</v>
       </c>
       <c r="M11" s="27">
-        <v>50000</v>
+        <v>68943</v>
       </c>
       <c r="N11" s="18">
         <v>30</v>
@@ -2238,12 +2262,12 @@
       <c r="P11" s="18">
         <v>0.7</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <f>P11</f>
         <v>0.7</v>
       </c>
     </row>
-    <row r="12" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C12" s="19" t="str">
         <f>'SATIM-EL'!H9</f>
         <v>ETGASGeneric</v>
@@ -2269,10 +2293,10 @@
         <v>1</v>
       </c>
       <c r="L12" s="18">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="M12" s="27">
-        <v>15000</v>
+        <v>12304</v>
       </c>
       <c r="N12" s="18">
         <v>30</v>
@@ -2283,12 +2307,12 @@
       <c r="P12" s="18">
         <v>0.9</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <f>P12</f>
         <v>0.9</v>
       </c>
     </row>
-    <row r="13" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>28</v>
       </c>
@@ -2299,11 +2323,12 @@
       <c r="F13" t="s">
         <v>11</v>
       </c>
-      <c r="L13">
-        <v>955</v>
+      <c r="L13" s="30">
+        <f>2%*M13</f>
+        <v>495.94</v>
       </c>
       <c r="M13" s="28">
-        <v>25000</v>
+        <v>24797</v>
       </c>
       <c r="N13">
         <v>20</v>
@@ -2311,15 +2336,15 @@
       <c r="O13" s="18">
         <v>31.536000000000001</v>
       </c>
-      <c r="S13">
-        <v>35.299999999999997</v>
-      </c>
-      <c r="T13" s="31">
-        <f>(-PMT($T$1,N13,1,0,1)*M13+L13)/S13</f>
-        <v>94.715730649564591</v>
-      </c>
-    </row>
-    <row r="14" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="T13" s="29">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="U13" s="30">
+        <f>(-PMT($U$1,N13,1,0,1)*M13+L13)/(T13*8.76)</f>
+        <v>926.50437662797719</v>
+      </c>
+    </row>
+    <row r="14" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>91</v>
       </c>
@@ -2330,11 +2355,12 @@
       <c r="F14" t="s">
         <v>11</v>
       </c>
-      <c r="L14">
-        <v>295</v>
+      <c r="L14" s="31">
+        <f>2%*M14</f>
+        <v>338</v>
       </c>
       <c r="M14" s="28">
-        <v>14000</v>
+        <v>16900</v>
       </c>
       <c r="N14">
         <v>25</v>
@@ -2342,15 +2368,15 @@
       <c r="O14" s="18">
         <v>31.536000000000001</v>
       </c>
-      <c r="S14">
-        <v>29.4</v>
-      </c>
-      <c r="T14" s="31">
-        <f>(-PMT($T$1,N14,1,0,1)*M14+L14)/S14</f>
-        <v>51.968852532769347</v>
-      </c>
-    </row>
-    <row r="15" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="T14" s="29">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="U14" s="30">
+        <f>(-PMT($U$1,N14,1,0,1)*M14+L14)/(T14*8.76)</f>
+        <v>709.10890315085635</v>
+      </c>
+    </row>
+    <row r="15" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C15" t="str">
         <f>Declarations!J19</f>
         <v>ESTGeneric</v>
@@ -2362,24 +2388,59 @@
       <c r="E15" t="s">
         <v>11</v>
       </c>
-      <c r="F15" t="s">
-        <v>11</v>
+      <c r="G15" t="s">
+        <v>50</v>
       </c>
       <c r="I15">
         <v>0.89</v>
       </c>
       <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="L15" s="31">
+        <f>3%*M15</f>
+        <v>855</v>
+      </c>
+      <c r="M15" s="28">
+        <v>28500</v>
+      </c>
+      <c r="N15">
+        <v>15</v>
+      </c>
+      <c r="O15" s="18">
+        <v>31.536000000000001</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="V15" s="30">
+        <f>-PMT($U$1,N15,1,0,1)*M15</f>
+        <v>3114.9852054439589</v>
+      </c>
+      <c r="W15" s="30">
+        <f>-PMT($U$1,N15,1,0,0)*M15</f>
+        <v>3370.4139922903632</v>
+      </c>
+      <c r="X15" s="30">
+        <f>V15*1.285</f>
+        <v>4002.7559889954869</v>
+      </c>
+      <c r="Y15" s="30">
+        <f>W15*1.285</f>
+        <v>4330.9819800931164</v>
+      </c>
+      <c r="Z15" s="30">
+        <f>(Y15+X15)/2</f>
+        <v>4166.8689845443014</v>
+      </c>
+    </row>
+    <row r="16" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>100</v>
+      </c>
+      <c r="J16">
         <f>4/24</f>
         <v>0.16666666666666666</v>
-      </c>
-      <c r="M15">
-        <v>19444</v>
-      </c>
-      <c r="N15">
-        <v>15</v>
-      </c>
-      <c r="O15" s="18">
-        <v>31.536000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Battery costs lowered so it enters solution
</commit_message>
<xml_diff>
--- a/VT_REGION1_PWR.xlsx
+++ b/VT_REGION1_PWR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\minimodel2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BC50C3-CC69-4612-93DB-2E8F50E43F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3E1425-7536-47F0-8C10-79AEE1ECAE5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1845" yWindow="-18225" windowWidth="28800" windowHeight="15570" activeTab="2" xr2:uid="{37FD0756-6F24-4C61-AC4B-6F35E5E0357A}"/>
+    <workbookView xWindow="1100" yWindow="1100" windowWidth="21600" windowHeight="12680" activeTab="2" xr2:uid="{37FD0756-6F24-4C61-AC4B-6F35E5E0357A}"/>
   </bookViews>
   <sheets>
     <sheet name="SATIM-EL" sheetId="2" r:id="rId1"/>
@@ -1232,24 +1232,24 @@
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="3.85546875" customWidth="1"/>
-    <col min="5" max="5" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" customWidth="1"/>
+    <col min="3" max="3" width="20.7265625" customWidth="1"/>
+    <col min="4" max="4" width="3.81640625" customWidth="1"/>
+    <col min="5" max="5" width="3.54296875" customWidth="1"/>
     <col min="6" max="7" width="4" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" customWidth="1"/>
-    <col min="9" max="9" width="3.5703125" customWidth="1"/>
-    <col min="10" max="10" width="3.85546875" customWidth="1"/>
-    <col min="11" max="11" width="22.5703125" customWidth="1"/>
-    <col min="12" max="12" width="3.5703125" customWidth="1"/>
-    <col min="13" max="13" width="3.85546875" customWidth="1"/>
-    <col min="14" max="14" width="22.5703125" customWidth="1"/>
-    <col min="15" max="15" width="3.5703125" customWidth="1"/>
+    <col min="8" max="8" width="23.1796875" customWidth="1"/>
+    <col min="9" max="9" width="3.54296875" customWidth="1"/>
+    <col min="10" max="10" width="3.81640625" customWidth="1"/>
+    <col min="11" max="11" width="22.54296875" customWidth="1"/>
+    <col min="12" max="12" width="3.54296875" customWidth="1"/>
+    <col min="13" max="13" width="3.81640625" customWidth="1"/>
+    <col min="14" max="14" width="22.54296875" customWidth="1"/>
+    <col min="15" max="15" width="3.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:15" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:15" ht="105.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="3:15" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:15" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C2" s="1"/>
       <c r="E2" s="2" t="s">
         <v>9</v>
@@ -1301,7 +1301,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:15" x14ac:dyDescent="0.35">
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="1"/>
@@ -1311,7 +1311,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="4"/>
     </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:15" x14ac:dyDescent="0.35">
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="1"/>
@@ -1321,7 +1321,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="4"/>
     </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:15" x14ac:dyDescent="0.35">
       <c r="D5" s="1"/>
       <c r="E5" s="4"/>
       <c r="F5" s="5"/>
@@ -1335,7 +1335,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="9"/>
     </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="4"/>
@@ -1356,7 +1356,7 @@
       </c>
       <c r="O6" s="6"/>
     </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C7" s="7" t="s">
         <v>18</v>
       </c>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="O7" s="7"/>
     </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C8" s="5" t="s">
         <v>21</v>
       </c>
@@ -1393,7 +1393,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="4"/>
     </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="4"/>
@@ -1408,7 +1408,7 @@
       <c r="N9" s="1"/>
       <c r="O9" s="4"/>
     </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="4"/>
@@ -1420,7 +1420,7 @@
       <c r="N10" s="1"/>
       <c r="O10" s="4"/>
     </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="4"/>
@@ -1435,7 +1435,7 @@
       <c r="N11" s="1"/>
       <c r="O11" s="4"/>
     </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="4"/>
@@ -1450,7 +1450,7 @@
       <c r="N12" s="1"/>
       <c r="O12" s="4"/>
     </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="4"/>
@@ -1462,7 +1462,7 @@
       <c r="N13" s="1"/>
       <c r="O13" s="4"/>
     </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="4"/>
@@ -1476,7 +1476,7 @@
       <c r="N14" s="1"/>
       <c r="O14" s="4"/>
     </row>
-    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="4"/>
@@ -1490,7 +1490,7 @@
       <c r="N15" s="1"/>
       <c r="O15" s="4"/>
     </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="4"/>
@@ -1501,7 +1501,7 @@
       <c r="N16" s="1"/>
       <c r="O16" s="4"/>
     </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:15" x14ac:dyDescent="0.35">
       <c r="E17" s="4"/>
       <c r="F17" s="14"/>
       <c r="H17" s="7" t="s">
@@ -1513,7 +1513,7 @@
       <c r="N17" s="1"/>
       <c r="O17" s="4"/>
     </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:15" x14ac:dyDescent="0.35">
       <c r="E18" s="4"/>
       <c r="F18" s="14"/>
       <c r="H18" s="5" t="s">
@@ -1525,7 +1525,7 @@
       <c r="N18" s="1"/>
       <c r="O18" s="4"/>
     </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:15" x14ac:dyDescent="0.35">
       <c r="E19" s="4"/>
       <c r="F19" s="14"/>
       <c r="I19" s="4"/>
@@ -1534,7 +1534,7 @@
       <c r="N19" s="1"/>
       <c r="O19" s="4"/>
     </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:15" x14ac:dyDescent="0.35">
       <c r="F20" s="14"/>
       <c r="H20" s="7" t="s">
         <v>90</v>
@@ -1545,7 +1545,7 @@
       <c r="N20" s="1"/>
       <c r="O20" s="4"/>
     </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C21" s="7" t="s">
         <v>29</v>
       </c>
@@ -1561,7 +1561,7 @@
       <c r="N21" s="1"/>
       <c r="O21" s="4"/>
     </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C22" s="5" t="s">
         <v>30</v>
       </c>
@@ -1574,7 +1574,7 @@
       <c r="N22" s="1"/>
       <c r="O22" s="4"/>
     </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:15" x14ac:dyDescent="0.35">
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="I23" s="4"/>
@@ -1583,7 +1583,7 @@
       <c r="N23" s="1"/>
       <c r="O23" s="4"/>
     </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:15" x14ac:dyDescent="0.35">
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="I24" s="4"/>
@@ -1592,7 +1592,7 @@
       <c r="N24" s="1"/>
       <c r="O24" s="4"/>
     </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:15" x14ac:dyDescent="0.35">
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="I25" s="4"/>
@@ -1616,23 +1616,23 @@
       <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" customWidth="1"/>
+    <col min="10" max="10" width="14.1796875" customWidth="1"/>
+    <col min="11" max="11" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C3" s="15" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="15"/>
     </row>
-    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C4" s="15" t="s">
         <v>32</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
         <v>9</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>10</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>11</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>12</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>13</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:16" x14ac:dyDescent="0.35">
       <c r="J10" t="s">
         <v>43</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:16" x14ac:dyDescent="0.35">
       <c r="J11" t="s">
         <v>21</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:16" x14ac:dyDescent="0.35">
       <c r="J12" t="s">
         <v>30</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:16" x14ac:dyDescent="0.35">
       <c r="J13" t="s">
         <v>19</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:16" x14ac:dyDescent="0.35">
       <c r="J14" t="s">
         <v>20</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:16" x14ac:dyDescent="0.35">
       <c r="J15" t="s">
         <v>15</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:16" x14ac:dyDescent="0.35">
       <c r="J16" t="s">
         <v>23</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="10:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="10:16" x14ac:dyDescent="0.35">
       <c r="J17" t="s">
         <v>28</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="10:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="10:16" x14ac:dyDescent="0.35">
       <c r="J18" t="s">
         <v>91</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="10:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="10:16" x14ac:dyDescent="0.35">
       <c r="J19" t="str">
         <f>'SATIM-EL'!H12</f>
         <v>ESTGeneric</v>
@@ -1979,24 +1979,24 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF44DDC-D079-43BE-BBFD-41A34FD9B05F}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="C1:Z16"/>
+  <dimension ref="C1:AB16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" customWidth="1"/>
-    <col min="20" max="20" width="11.140625" customWidth="1"/>
-    <col min="21" max="25" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" customWidth="1"/>
+    <col min="13" max="13" width="11.453125" customWidth="1"/>
+    <col min="14" max="14" width="11.1796875" customWidth="1"/>
+    <col min="15" max="15" width="12.1796875" customWidth="1"/>
+    <col min="20" max="20" width="11.1796875" customWidth="1"/>
+    <col min="21" max="25" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:28" x14ac:dyDescent="0.35">
       <c r="S1" t="s">
         <v>92</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="3" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:28" x14ac:dyDescent="0.35">
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
@@ -2020,7 +2020,7 @@
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
     </row>
-    <row r="4" spans="3:26" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:28" ht="21.5" x14ac:dyDescent="0.35">
       <c r="C4" s="21" t="s">
         <v>43</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:28" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
         <v>70</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:28" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>78</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:28" x14ac:dyDescent="0.35">
       <c r="C7" t="str">
         <f>'SATIM-EL'!C8</f>
         <v>MINCLE</v>
@@ -2148,7 +2148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:28" x14ac:dyDescent="0.35">
       <c r="C8" t="str">
         <f>'SATIM-EL'!C22</f>
         <v>IMPGAS</v>
@@ -2170,7 +2170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:28" x14ac:dyDescent="0.35">
       <c r="C9" t="str">
         <f>'SATIM-EL'!K7</f>
         <v>ETRANS</v>
@@ -2198,7 +2198,7 @@
         <v>31.536000000000001</v>
       </c>
     </row>
-    <row r="10" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:28" x14ac:dyDescent="0.35">
       <c r="C10" t="str">
         <f>'SATIM-EL'!N7</f>
         <v>RDEM</v>
@@ -2222,7 +2222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:28" x14ac:dyDescent="0.35">
       <c r="C11" s="19" t="str">
         <f>'SATIM-EL'!H6</f>
         <v>ETCLEGeneric</v>
@@ -2267,7 +2267,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="12" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:28" x14ac:dyDescent="0.35">
       <c r="C12" s="19" t="str">
         <f>'SATIM-EL'!H9</f>
         <v>ETGASGeneric</v>
@@ -2312,7 +2312,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="13" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:28" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>28</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>926.50437662797719</v>
       </c>
     </row>
-    <row r="14" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:28" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>91</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>709.10890315085635</v>
       </c>
     </row>
-    <row r="15" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:28" x14ac:dyDescent="0.35">
       <c r="C15" t="str">
         <f>Declarations!J19</f>
         <v>ESTGeneric</v>
@@ -2399,10 +2399,10 @@
       </c>
       <c r="L15" s="31">
         <f>3%*M15</f>
-        <v>855</v>
+        <v>300</v>
       </c>
       <c r="M15" s="28">
-        <v>28500</v>
+        <v>10000</v>
       </c>
       <c r="N15">
         <v>15</v>
@@ -2415,26 +2415,29 @@
       </c>
       <c r="V15" s="30">
         <f>-PMT($U$1,N15,1,0,1)*M15</f>
-        <v>3114.9852054439589</v>
+        <v>1092.9772650680557</v>
       </c>
       <c r="W15" s="30">
         <f>-PMT($U$1,N15,1,0,0)*M15</f>
-        <v>3370.4139922903632</v>
+        <v>1182.6014008036361</v>
       </c>
       <c r="X15" s="30">
         <f>V15*1.285</f>
-        <v>4002.7559889954869</v>
+        <v>1404.4757856124515</v>
       </c>
       <c r="Y15" s="30">
         <f>W15*1.285</f>
-        <v>4330.9819800931164</v>
+        <v>1519.6428000326723</v>
       </c>
       <c r="Z15" s="30">
         <f>(Y15+X15)/2</f>
-        <v>4166.8689845443014</v>
-      </c>
-    </row>
-    <row r="16" spans="3:26" x14ac:dyDescent="0.25">
+        <v>1462.0592928225619</v>
+      </c>
+      <c r="AB15" s="28">
+        <v>28500</v>
+      </c>
+    </row>
+    <row r="16" spans="3:28" x14ac:dyDescent="0.35">
       <c r="G16" t="s">
         <v>100</v>
       </c>
@@ -2457,12 +2460,12 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C3" s="15"/>
       <c r="D3" s="15" t="s">
         <v>59</v>
@@ -2470,7 +2473,7 @@
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C4" s="15" t="s">
         <v>82</v>
       </c>
@@ -2484,7 +2487,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C5" s="24" t="s">
         <v>78</v>
       </c>
@@ -2498,7 +2501,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C6" s="24" t="s">
         <v>87</v>
       </c>
@@ -2508,7 +2511,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C7" s="24" t="s">
         <v>88</v>
       </c>

</xml_diff>